<commit_message>
reactivated several unit tests + fixed several issues
</commit_message>
<xml_diff>
--- a/ExcelOpsTest/test_data/ExcelOpsGrund01.xlsx
+++ b/ExcelOpsTest/test_data/ExcelOpsGrund01.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-OpenSource-Externals+Backups\CompuMaster.Excel\ExcelOpsTest\test_data\ctworkbook_masters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-OpenSource-Externals+Backups\CompuMaster.Excel\ExcelOpsTest\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A842DF71-9A13-4E50-B920-2081B6E464DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E24709-5960-4E3A-88D9-B638133C3C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="937" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grunddaten" sheetId="29" r:id="rId1"/>
+    <sheet name="Kostenplanung" sheetId="30" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Bildbereich">#REF!</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Januar</t>
   </si>
@@ -128,6 +129,21 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Kostenplanung</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Sonstige</t>
+  </si>
+  <si>
+    <t>Summe</t>
   </si>
 </sst>
 </file>
@@ -136,13 +152,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="0_)"/>
-    <numFmt numFmtId="182" formatCode="&quot;Chef: &quot;0.00"/>
-    <numFmt numFmtId="183" formatCode="&quot;Büroangestellte: &quot;0.00"/>
-    <numFmt numFmtId="184" formatCode="&quot;Produktivkraft: &quot;0.00"/>
-    <numFmt numFmtId="185" formatCode="&quot;Azubi / Aushilfen: &quot;0.00"/>
+    <numFmt numFmtId="165" formatCode="0_)"/>
+    <numFmt numFmtId="166" formatCode="&quot;Chef: &quot;0.00"/>
+    <numFmt numFmtId="167" formatCode="&quot;Büroangestellte: &quot;0.00"/>
+    <numFmt numFmtId="168" formatCode="&quot;Produktivkraft: &quot;0.00"/>
+    <numFmt numFmtId="169" formatCode="&quot;Azubi / Aushilfen: &quot;0.00"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -253,9 +269,19 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="MS Sans Serif"/>
-      <family val="2"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -290,7 +316,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -335,8 +361,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
@@ -351,7 +388,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="6" fillId="1" borderId="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="6" fillId="1" borderId="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -397,8 +434,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -410,24 +449,29 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="17" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="182" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="183" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="184" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="185" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="27"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="26" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="28">
     <cellStyle name="1Tabellentext" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="2Tabellentext fett" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="3Tabellentext Zeilenfall" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="4Tabellentext fett Zeilenfall" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Ergebnis" xfId="27" builtinId="25"/>
     <cellStyle name="Komma 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Kopfzeile" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Muster 1" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -442,6 +486,7 @@
     <cellStyle name="Standard fett_Anwenderhilfe" xfId="10" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Standard Zeilenfall" xfId="11" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Titel" xfId="12" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Überschrift" xfId="26" builtinId="15"/>
     <cellStyle name="Überschrift 1" xfId="13" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 2" xfId="14" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Überschrift 2 Diagramm" xfId="15" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
@@ -821,10 +866,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -836,15 +881,18 @@
     <col min="8" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="3">
         <v>2019</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -854,7 +902,7 @@
       </c>
       <c r="D2" s="8"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
@@ -866,10 +914,10 @@
         <v>Januar</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
@@ -877,37 +925,37 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>14.09</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -915,7 +963,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -924,7 +972,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>16</v>
       </c>
@@ -1102,4 +1150,64 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1292CE-2C96-4FCD-B0CD-6AACA376EB74}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
+        <f>Grunddaten!B1</f>
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="13">
+        <f>SUM(B4:B6)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>